<commit_message>
feat: update of dependencies to add support for 'distinct' function by definition name
also add dashboard-info lib as es module
</commit_message>
<xml_diff>
--- a/others/customize.dashboard.dash/instances/2.dashboard_v1.xlsx
+++ b/others/customize.dashboard.dash/instances/2.dashboard_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguelmesquita/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguelmesquita/.local/share/cob-cli/customize.dashboard.dash/others/customize.dashboard.dash/instances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A094630A-C990-B542-A34A-3F197159EF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26110BA0-BDB3-1D43-A655-7BE95C15B3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22720" yWindow="9580" windowWidth="28620" windowHeight="19340" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -611,27 +611,27 @@
     <t>#/cob.custom-resource/SOLUTION:{"arg":"{{sigla}}"}/dash</t>
   </si>
   <si>
+    <t>SERVER NAME</t>
+  </si>
+  <si>
+    <t>Files Def Id</t>
+  </si>
+  <si>
+    <t>Dashboard Attention Def Id:</t>
+  </si>
+  <si>
+    <t>Dashboard Def Id:</t>
+  </si>
+  <si>
+    <t>Server Name:</t>
+  </si>
+  <si>
+    <t>Solutions Def Id</t>
+  </si>
+  <si>
     <t>{
-   "dashs": distinct(89, "solution", 'solution:* (groupaccess.raw:( {{user.groupsQuery}} ) OR (-groupaccess:*) )',  90, { validity: 600 })
+   "dashs": distinct("Dashboard_v1", "solution", 'solution:* (groupaccess.raw:( {{user.groupsQuery}} ) OR (-groupaccess:*) )',  90, { validity: 600 })
 }</t>
-  </si>
-  <si>
-    <t>SERVER NAME</t>
-  </si>
-  <si>
-    <t>Files Def Id</t>
-  </si>
-  <si>
-    <t>Dashboard Attention Def Id:</t>
-  </si>
-  <si>
-    <t>Dashboard Def Id:</t>
-  </si>
-  <si>
-    <t>Server Name:</t>
-  </si>
-  <si>
-    <t>Solutions Def Id</t>
   </si>
 </sst>
 </file>
@@ -1018,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1109,7 +1109,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-2</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="H3" t="s">
         <v>22</v>
@@ -1923,7 +1923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
@@ -2666,15 +2666,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -2682,7 +2682,7 @@
     </row>
     <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -2690,7 +2690,7 @@
     </row>
     <row r="4" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -2698,7 +2698,7 @@
     </row>
     <row r="5" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>

</xml_diff>